<commit_message>
Updated Boxplots and shortend df names to clean up code.
</commit_message>
<xml_diff>
--- a/output_file.xlsx
+++ b/output_file.xlsx
@@ -604,19 +604,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>52.39346338487179</v>
+        <v>52.32092986</v>
       </c>
       <c r="C8" t="n">
-        <v>50.909964985</v>
+        <v>50.446266345</v>
       </c>
       <c r="D8" t="n">
-        <v>43.13880349780112</v>
+        <v>43.85201301302044</v>
       </c>
       <c r="E8" t="n">
-        <v>6.568013664556516</v>
+        <v>6.62208524658362</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5258619511360096</v>
+        <v>0.544332054194047</v>
       </c>
     </row>
     <row r="9">

</xml_diff>